<commit_message>
Gestiona min y mayus campos strings. Campos numericos >0. Vinculo posiicon rack con rack y posicion caja con caja. No permite subir posiciones si hay errores.
</commit_message>
<xml_diff>
--- a/datos_prueba/globalstaticfiles/plantilla_localizaciones.xlsx
+++ b/datos_prueba/globalstaticfiles/plantilla_localizaciones.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthem\Desktop\programas_python\datos_prueba\datos_prueba\globalstaticfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive\Documentos\Practicas_UOC\datos_muestras\datos_prueba\globalstaticfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB715A04-6675-46A9-8633-3CDDDCD7CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC2ADA6-480E-4A6B-A995-7163877AE88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="14355" windowHeight="15480" xr2:uid="{2909E318-E7CF-4341-AC61-03CBD1DEEF01}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2909E318-E7CF-4341-AC61-03CBD1DEEF01}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ubicaciones" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,9 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -122,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -162,7 +159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -268,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -410,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -424,14 +421,14 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.26953125" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>